<commit_message>
Accurate and complete report generation done!
</commit_message>
<xml_diff>
--- a/comparison_report.xlsx
+++ b/comparison_report.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/all/south-africa</t>
+          <t>https://www.varoom.com/all/puerto-rico</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,22 +503,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>rating</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>৳54,694</t>
+          <t>New</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>৳54,694</t>
+          <t>New</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>৳54,694</t>
+          <t>New</t>
         </is>
       </c>
       <c r="I2" t="b">
@@ -533,7 +533,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/all/south-africa</t>
+          <t>https://www.varoom.com/all/puerto-rico</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -548,22 +548,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>rating</t>
+          <t>number_of_reviews</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>New</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>New</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>New</t>
         </is>
       </c>
       <c r="I3" t="b">
@@ -578,7 +578,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/all/south-africa</t>
+          <t>https://www.varoom.com/all/puerto-rico</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -593,22 +593,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>number_of_reviews</t>
+          <t>property_type</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(70 Reviews)</t>
+          <t>Apartment</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(70 Reviews)</t>
+          <t>Apartment</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(70 Reviews)</t>
+          <t>Apartment</t>
         </is>
       </c>
       <c r="I4" t="b">
@@ -623,7 +623,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/all/south-africa</t>
+          <t>https://www.varoom.com/all/puerto-rico</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -638,22 +638,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>property_type</t>
+          <t>title</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>House</t>
+          <t>Newly Furnished 3 Bedroom Apartment 1 Bath in Hato Rey San Juan Puerto Rico</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>House</t>
+          <t>Newly Furnished 3 Bedroom Apartment 1 Bath in Hato Rey San Juan Puerto Rico</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>House</t>
+          <t>Newly Furnished 3 Bedroom Apartment 1 Bath in Hato Rey San Juan Puerto Rico</t>
         </is>
       </c>
       <c r="I5" t="b">
@@ -668,7 +668,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/all/south-africa</t>
+          <t>https://www.varoom.com/all/puerto-rico</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -683,26 +683,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>price</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Pure Sea Boutique Lodge</t>
+          <t>৳14,590</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pure Sea Boutique Lodge</t>
+          <t>৳14,590</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Pure Sea Boutique Lodge | House in Gansbaai</t>
+          <t>৳14,590</t>
         </is>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>